<commit_message>
@Ioannis E. Kommas (PyCharm Commit and Push Code Lines) All Rights Reserved (Private Repository)
</commit_message>
<xml_diff>
--- a/A_DAILY_ΠΟΡΕΙΑ_ΤΙΜΟΚΑΤΑΛΟΓΟΥ_ΠΩΛΗΣΕΩΝ/excel/15.xlsx
+++ b/A_DAILY_ΠΟΡΕΙΑ_ΤΙΜΟΚΑΤΑΛΟΓΟΥ_ΠΩΛΗΣΕΩΝ/excel/15.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
   <si>
     <t>ΤΙΜΟΚΑΤΑΛΟΓΟΣ</t>
   </si>
@@ -52,16 +52,241 @@
     <t>Turnover</t>
   </si>
   <si>
+    <t>Πωλήσεις Έκπτωση 1</t>
+  </si>
+  <si>
     <t>Πελάτες Τιμή Πώλησης</t>
   </si>
   <si>
+    <t>Selpak® Toilet Paper Ocean 8τεμ.</t>
+  </si>
+  <si>
+    <t>Bazaar® Υγρό Πατώματος Ultra Άνθη Πασχαλιάς 1ltr</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Repair &amp; Protect 360ml</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Classic 360ml</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Aqqa Light 400ml</t>
+  </si>
+  <si>
+    <t>Nutella® Πραλίνα Βάζο 400gr</t>
+  </si>
+  <si>
+    <t>NEOMAT 2,25KG ΣΚΟΝΗ ΜΠΛΕ  /45ΜΕΖ</t>
+  </si>
+  <si>
+    <t>NEOMAT 2,25KG ΣΚΟΝΗ ΑΓΡΙΟ ΤΡΙΑΝΤΑΦΥΛΛΟ / 45ΜΕΖ</t>
+  </si>
+  <si>
+    <t>Kelloggs® Δημητριακά Coco Pops White Choco 375gr</t>
+  </si>
+  <si>
+    <t>3 Άλφα® Φασόλια Γίγαντες 500gr</t>
+  </si>
+  <si>
+    <t>Selpak® Toilet Paper Levander 8τεμ.</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Τελειες Μπουκλες 360ml</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Πλουσιο Ογκο 360ml</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Hydration 360ml</t>
+  </si>
+  <si>
+    <t>NEOMAT 2,1L GEL ΜΑΛΑΙΣΙΑΝΗ ΟΡΧΙΔ. &amp; ΣΑΝΔΑΛ. / 42 ΜΕΖ</t>
+  </si>
+  <si>
+    <t>Farmer® Ρύζι Τύπου Αμερικής 1kgr</t>
+  </si>
+  <si>
+    <t>Bazaar® Υγρό Γεν. Καθαρισμού Μπουκέτο Λουλουδιών 1ltr</t>
+  </si>
+  <si>
+    <t>Colgate® Οδοντόκρεμα Triple Action 100ml</t>
+  </si>
+  <si>
+    <t>NEOMAT 2,1L GEL 2ΣΕ1 ΑΕΡΙΝΗ ΦΡΕΣΚ / 42 ΜΕΖ</t>
+  </si>
+  <si>
+    <t>Colgate® Max Fresh Cool Mint 100gr</t>
+  </si>
+  <si>
+    <t>Selpak® Toilet Paper Powder 8τεμ.</t>
+  </si>
+  <si>
+    <t>Bazaar® Καθαριστικό Άρωμα Φρεσκάδας Plus 1ltr</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Smooth &amp; Sleek 360ml</t>
+  </si>
+  <si>
+    <t>Colgate® Deep Clean Whitening 100ml</t>
+  </si>
+  <si>
+    <t>Dixan® Gel Πλυντηριου Clean Smooth 42μεζ.</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Colour Protect 360ml</t>
+  </si>
+  <si>
+    <t>DIXAN 2L GEL CLEAN &amp; SMOOTH / 40ΜΕΖ</t>
+  </si>
+  <si>
+    <t>AVA PERLE 430ML CLASSIC</t>
+  </si>
+  <si>
     <t>Παπαγάλος® Greek Premium Coffee 194gr</t>
   </si>
   <si>
+    <t>AVA PERLE 430ML ΛΕΜΟΝΙ</t>
+  </si>
+  <si>
+    <t>Colgate® Οδοντόκρεμα Advance White 75ml</t>
+  </si>
+  <si>
+    <t>Royal Dutch® Μπύρα Κουτί 330ml</t>
+  </si>
+  <si>
+    <t>8690530044494</t>
+  </si>
+  <si>
+    <t>5208086416820</t>
+  </si>
+  <si>
+    <t>4015600948016</t>
+  </si>
+  <si>
+    <t>4084500290532</t>
+  </si>
+  <si>
+    <t>8001090724984</t>
+  </si>
+  <si>
+    <t>80135876</t>
+  </si>
+  <si>
+    <t>5201395136939</t>
+  </si>
+  <si>
+    <t>5201395137134</t>
+  </si>
+  <si>
+    <t>5053827215671</t>
+  </si>
+  <si>
+    <t>5201399010235</t>
+  </si>
+  <si>
+    <t>8690530044500</t>
+  </si>
+  <si>
+    <t>4084500290242</t>
+  </si>
+  <si>
+    <t>4084500290570</t>
+  </si>
+  <si>
+    <t>4084500929982</t>
+  </si>
+  <si>
+    <t>5201395137530</t>
+  </si>
+  <si>
+    <t>5208086412464</t>
+  </si>
+  <si>
+    <t>5208086420353</t>
+  </si>
+  <si>
+    <t>7891024132074</t>
+  </si>
+  <si>
+    <t>5201395133334</t>
+  </si>
+  <si>
+    <t>8850006324172</t>
+  </si>
+  <si>
+    <t>8690530044517</t>
+  </si>
+  <si>
+    <t>5208086416387</t>
+  </si>
+  <si>
+    <t>4084500290600</t>
+  </si>
+  <si>
+    <t>8714789115474</t>
+  </si>
+  <si>
+    <t>5201395138339</t>
+  </si>
+  <si>
+    <t>4084500929951</t>
+  </si>
+  <si>
+    <t>5201395138438</t>
+  </si>
+  <si>
+    <t>5201314120902</t>
+  </si>
+  <si>
     <t>5201219486417</t>
   </si>
   <si>
+    <t>5201314120926</t>
+  </si>
+  <si>
+    <t>6001067003366</t>
+  </si>
+  <si>
+    <t>87250510</t>
+  </si>
+  <si>
+    <t>Selpak</t>
+  </si>
+  <si>
+    <t>Bazaar</t>
+  </si>
+  <si>
+    <t>Pantene</t>
+  </si>
+  <si>
+    <t>Nutella</t>
+  </si>
+  <si>
+    <t>Neomat</t>
+  </si>
+  <si>
+    <t>Kelloggs</t>
+  </si>
+  <si>
+    <t>3 Άλφα</t>
+  </si>
+  <si>
+    <t>Farmer</t>
+  </si>
+  <si>
+    <t>Colgate</t>
+  </si>
+  <si>
+    <t>Dixan</t>
+  </si>
+  <si>
+    <t>Ava</t>
+  </si>
+  <si>
     <t>Παπαγάλος</t>
+  </si>
+  <si>
+    <t>Royal Dutch</t>
   </si>
 </sst>
 </file>
@@ -446,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -509,46 +734,1131 @@
         <v>12</v>
       </c>
       <c r="C2" s="4">
-        <v>43988</v>
+        <v>43998</v>
       </c>
       <c r="D2" s="4">
-        <v>43997</v>
+        <v>44012</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3.15</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="C3" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.15</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D4" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D5" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D6" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D7" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3.78</v>
+      </c>
+      <c r="H7" s="2">
         <v>2.95</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D8" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="2">
+        <v>8.949999999999999</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5.59</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D9" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8.949999999999999</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5.59</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D10" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>50</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D11" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3.45</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.69</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D12" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3.35</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D13" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>30</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D14" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D15" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>30</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D16" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5.59</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D17" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D18" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.15</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D19" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2.95</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>50</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D20" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5.59</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D21" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>50</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D22" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3.35</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>30</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K22" s="1">
+        <v>2</v>
+      </c>
+      <c r="L22" s="2">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D23" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.15</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K23" s="1">
+        <v>2</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D24" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>30</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" s="1">
+        <v>2</v>
+      </c>
+      <c r="L24" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D25" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>50</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K25" s="1">
+        <v>2</v>
+      </c>
+      <c r="L25" s="2">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D26" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="2">
+        <v>7.95</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>30</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K26" s="1">
+        <v>2</v>
+      </c>
+      <c r="L26" s="2">
+        <v>8.98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D27" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="2">
+        <v>3.98</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>30</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K27" s="1">
+        <v>2</v>
+      </c>
+      <c r="L27" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D28" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="2">
+        <v>7.95</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>30</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K28" s="1">
+        <v>3</v>
+      </c>
+      <c r="L28" s="2">
+        <v>13.47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D29" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>30</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K29" s="1">
+        <v>3</v>
+      </c>
+      <c r="L29" s="2">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D30" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2.95</v>
+      </c>
+      <c r="H30" s="2">
         <v>2.29</v>
       </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K30" s="1">
+        <v>3</v>
+      </c>
+      <c r="L30" s="2">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D31" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>30</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K31" s="1">
         <v>5</v>
       </c>
-      <c r="L2" s="2">
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="K3" s="5">
-        <v>5</v>
-      </c>
-      <c r="L3" s="5">
-        <v>10.15</v>
+      <c r="L31" s="2">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D32" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="2">
+        <v>2.95</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>50</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K32" s="1">
+        <v>7</v>
+      </c>
+      <c r="L32" s="2">
+        <v>7.97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="4">
+        <v>43998</v>
+      </c>
+      <c r="D33" s="4">
+        <v>44012</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K33" s="1">
+        <v>22</v>
+      </c>
+      <c r="L33" s="2">
+        <v>11.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="K34" s="5">
+        <v>66</v>
+      </c>
+      <c r="L34" s="5">
+        <v>93.11</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I2">
+  <conditionalFormatting sqref="I1:I33">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -560,7 +1870,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J2">
+  <conditionalFormatting sqref="J1:J33">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
@Ioannis E. Kommas (PyCharm Commit and Push Code Lines)
</commit_message>
<xml_diff>
--- a/A_DAILY_ΠΟΡΕΙΑ_ΤΙΜΟΚΑΤΑΛΟΓΟΥ_ΠΩΛΗΣΕΩΝ/excel/15.xlsx
+++ b/A_DAILY_ΠΟΡΕΙΑ_ΤΙΜΟΚΑΤΑΛΟΓΟΥ_ΠΩΛΗΣΕΩΝ/excel/15.xlsx
@@ -58,198 +58,198 @@
     <t>Πελάτες Τιμή Πώλησης</t>
   </si>
   <si>
+    <t>Pantene® Shampoo Classic 360ml</t>
+  </si>
+  <si>
+    <t>NEOMAT 2,25KG ΣΚΟΝΗ ΜΠΛΕ  /45ΜΕΖ</t>
+  </si>
+  <si>
+    <t>Selpak® Toilet Paper Ocean 8τεμ.</t>
+  </si>
+  <si>
     <t>Pantene® Shampoo Repair &amp; Protect 360ml</t>
   </si>
   <si>
-    <t>Pantene® Shampoo Classic 360ml</t>
-  </si>
-  <si>
-    <t>Selpak® Toilet Paper Ocean 8τεμ.</t>
-  </si>
-  <si>
     <t>Pantene® Shampoo Aqqa Light 400ml</t>
   </si>
   <si>
+    <t>Pantene® Shampoo Hydration 360ml</t>
+  </si>
+  <si>
+    <t>NEOMAT 2,1L GEL ΜΑΛΑΙΣΙΑΝΗ ΟΡΧΙΔ. &amp; ΣΑΝΔΑΛ. / 42 ΜΕΖ</t>
+  </si>
+  <si>
+    <t>NEOMAT 2,1L GEL 2ΣΕ1 ΑΕΡΙΝΗ ΦΡΕΣΚ / 42 ΜΕΖ</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Πλουσιο Ογκο 360ml</t>
+  </si>
+  <si>
+    <t>NEOMAT 2,25KG ΣΚΟΝΗ ΑΓΡΙΟ ΤΡΙΑΝΤΑΦΥΛΛΟ / 45ΜΕΖ</t>
+  </si>
+  <si>
+    <t>Colgate® Max Fresh Cool Mint 100gr</t>
+  </si>
+  <si>
     <t>Bazaar® Υγρό Πατώματος Ultra Άνθη Πασχαλιάς 1ltr</t>
   </si>
   <si>
-    <t>NEOMAT 2,25KG ΣΚΟΝΗ ΜΠΛΕ  /45ΜΕΖ</t>
+    <t>Colgate® Deep Clean Whitening 100ml</t>
+  </si>
+  <si>
+    <t>Farmer® Ρύζι Τύπου Αμερικής 1kgr</t>
+  </si>
+  <si>
+    <t>Kelloggs® Δημητριακά Coco Pops White Choco 375gr</t>
+  </si>
+  <si>
+    <t>Bazaar® Καθαριστικό Άρωμα Φρεσκάδας Plus 1ltr</t>
+  </si>
+  <si>
+    <t>Selpak® Toilet Paper Powder 8τεμ.</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Colour Protect 360ml</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Τελειες Μπουκλες 360ml</t>
+  </si>
+  <si>
+    <t>Pantene® Shampoo Smooth &amp; Sleek 360ml</t>
+  </si>
+  <si>
+    <t>Selpak® Toilet Paper Levander 8τεμ.</t>
+  </si>
+  <si>
+    <t>3 Άλφα® Φασόλια Γίγαντες 500gr</t>
+  </si>
+  <si>
+    <t>Dixan® Gel Πλυντηριου Clean Smooth 42μεζ.</t>
+  </si>
+  <si>
+    <t>DIXAN 2L GEL CLEAN &amp; SMOOTH / 40ΜΕΖ</t>
+  </si>
+  <si>
+    <t>Colgate® Οδοντόκρεμα Triple Action 100ml</t>
+  </si>
+  <si>
+    <t>Παπαγάλος® Greek Premium Coffee 194gr</t>
+  </si>
+  <si>
+    <t>Bazaar® Υγρό Γεν. Καθαρισμού Μπουκέτο Λουλουδιών 1ltr</t>
+  </si>
+  <si>
+    <t>AVA PERLE 430ML CLASSIC</t>
   </si>
   <si>
     <t>Nutella® Πραλίνα Βάζο 400gr</t>
   </si>
   <si>
+    <t>AVA PERLE 430ML ΛΕΜΟΝΙ</t>
+  </si>
+  <si>
     <t>Tasty® Lays Αλάτι 150gr</t>
   </si>
   <si>
-    <t>NEOMAT 2,1L GEL ΜΑΛΑΙΣΙΑΝΗ ΟΡΧΙΔ. &amp; ΣΑΝΔΑΛ. / 42 ΜΕΖ</t>
-  </si>
-  <si>
-    <t>NEOMAT 2,1L GEL 2ΣΕ1 ΑΕΡΙΝΗ ΦΡΕΣΚ / 42 ΜΕΖ</t>
-  </si>
-  <si>
-    <t>Farmer® Ρύζι Τύπου Αμερικής 1kgr</t>
-  </si>
-  <si>
-    <t>NEOMAT 2,25KG ΣΚΟΝΗ ΑΓΡΙΟ ΤΡΙΑΝΤΑΦΥΛΛΟ / 45ΜΕΖ</t>
-  </si>
-  <si>
-    <t>Pantene® Shampoo Πλουσιο Ογκο 360ml</t>
-  </si>
-  <si>
-    <t>Colgate® Max Fresh Cool Mint 100gr</t>
-  </si>
-  <si>
-    <t>Pantene® Shampoo Hydration 360ml</t>
-  </si>
-  <si>
-    <t>Pantene® Shampoo Smooth &amp; Sleek 360ml</t>
-  </si>
-  <si>
-    <t>Kelloggs® Δημητριακά Coco Pops White Choco 375gr</t>
-  </si>
-  <si>
-    <t>Pantene® Shampoo Τελειες Μπουκλες 360ml</t>
-  </si>
-  <si>
-    <t>Colgate® Deep Clean Whitening 100ml</t>
-  </si>
-  <si>
-    <t>Selpak® Toilet Paper Levander 8τεμ.</t>
-  </si>
-  <si>
-    <t>Bazaar® Καθαριστικό Άρωμα Φρεσκάδας Plus 1ltr</t>
-  </si>
-  <si>
-    <t>Selpak® Toilet Paper Powder 8τεμ.</t>
-  </si>
-  <si>
-    <t>Pantene® Shampoo Colour Protect 360ml</t>
-  </si>
-  <si>
-    <t>Dixan® Gel Πλυντηριου Clean Smooth 42μεζ.</t>
-  </si>
-  <si>
-    <t>3 Άλφα® Φασόλια Γίγαντες 500gr</t>
-  </si>
-  <si>
-    <t>Colgate® Οδοντόκρεμα Triple Action 100ml</t>
-  </si>
-  <si>
-    <t>DIXAN 2L GEL CLEAN &amp; SMOOTH / 40ΜΕΖ</t>
-  </si>
-  <si>
-    <t>Παπαγάλος® Greek Premium Coffee 194gr</t>
-  </si>
-  <si>
-    <t>Bazaar® Υγρό Γεν. Καθαρισμού Μπουκέτο Λουλουδιών 1ltr</t>
-  </si>
-  <si>
-    <t>AVA PERLE 430ML CLASSIC</t>
-  </si>
-  <si>
-    <t>AVA PERLE 430ML ΛΕΜΟΝΙ</t>
-  </si>
-  <si>
     <t>Colgate® Οδοντόκρεμα Advance White 75ml</t>
   </si>
   <si>
     <t>Royal Dutch® Μπύρα Κουτί 330ml</t>
   </si>
   <si>
+    <t>4084500290532</t>
+  </si>
+  <si>
+    <t>5201395136939</t>
+  </si>
+  <si>
+    <t>8690530044494</t>
+  </si>
+  <si>
     <t>4015600948016</t>
   </si>
   <si>
-    <t>4084500290532</t>
-  </si>
-  <si>
-    <t>8690530044494</t>
-  </si>
-  <si>
     <t>8001090724984</t>
   </si>
   <si>
+    <t>4084500929982</t>
+  </si>
+  <si>
+    <t>5201395137530</t>
+  </si>
+  <si>
+    <t>5201395133334</t>
+  </si>
+  <si>
+    <t>4084500290570</t>
+  </si>
+  <si>
+    <t>5201395137134</t>
+  </si>
+  <si>
+    <t>8850006324172</t>
+  </si>
+  <si>
     <t>5208086416820</t>
   </si>
   <si>
-    <t>5201395136939</t>
+    <t>8714789115474</t>
+  </si>
+  <si>
+    <t>5208086412464</t>
+  </si>
+  <si>
+    <t>5053827215671</t>
+  </si>
+  <si>
+    <t>5208086416387</t>
+  </si>
+  <si>
+    <t>8690530044517</t>
+  </si>
+  <si>
+    <t>4084500929951</t>
+  </si>
+  <si>
+    <t>4084500290242</t>
+  </si>
+  <si>
+    <t>4084500290600</t>
+  </si>
+  <si>
+    <t>8690530044500</t>
+  </si>
+  <si>
+    <t>5201399010235</t>
+  </si>
+  <si>
+    <t>5201395138339</t>
+  </si>
+  <si>
+    <t>5201395138438</t>
+  </si>
+  <si>
+    <t>7891024132074</t>
+  </si>
+  <si>
+    <t>5201219486417</t>
+  </si>
+  <si>
+    <t>5208086420353</t>
+  </si>
+  <si>
+    <t>5201314120902</t>
   </si>
   <si>
     <t>80135876</t>
   </si>
   <si>
+    <t>5201314120926</t>
+  </si>
+  <si>
     <t>5201024779957</t>
   </si>
   <si>
-    <t>5201395137530</t>
-  </si>
-  <si>
-    <t>5201395133334</t>
-  </si>
-  <si>
-    <t>5208086412464</t>
-  </si>
-  <si>
-    <t>5201395137134</t>
-  </si>
-  <si>
-    <t>4084500290570</t>
-  </si>
-  <si>
-    <t>8850006324172</t>
-  </si>
-  <si>
-    <t>4084500929982</t>
-  </si>
-  <si>
-    <t>4084500290600</t>
-  </si>
-  <si>
-    <t>5053827215671</t>
-  </si>
-  <si>
-    <t>4084500290242</t>
-  </si>
-  <si>
-    <t>8714789115474</t>
-  </si>
-  <si>
-    <t>8690530044500</t>
-  </si>
-  <si>
-    <t>5208086416387</t>
-  </si>
-  <si>
-    <t>8690530044517</t>
-  </si>
-  <si>
-    <t>4084500929951</t>
-  </si>
-  <si>
-    <t>5201395138339</t>
-  </si>
-  <si>
-    <t>5201399010235</t>
-  </si>
-  <si>
-    <t>7891024132074</t>
-  </si>
-  <si>
-    <t>5201395138438</t>
-  </si>
-  <si>
-    <t>5201219486417</t>
-  </si>
-  <si>
-    <t>5208086420353</t>
-  </si>
-  <si>
-    <t>5201314120902</t>
-  </si>
-  <si>
-    <t>5201314120926</t>
-  </si>
-  <si>
     <t>6001067003366</t>
   </si>
   <si>
@@ -259,40 +259,40 @@
     <t>Pantene</t>
   </si>
   <si>
+    <t>Neomat</t>
+  </si>
+  <si>
     <t>Selpak</t>
   </si>
   <si>
+    <t>Colgate</t>
+  </si>
+  <si>
     <t>Bazaar</t>
   </si>
   <si>
-    <t>Neomat</t>
+    <t>Farmer</t>
+  </si>
+  <si>
+    <t>Kelloggs</t>
+  </si>
+  <si>
+    <t>3 Άλφα</t>
+  </si>
+  <si>
+    <t>Dixan</t>
+  </si>
+  <si>
+    <t>Παπαγάλος</t>
+  </si>
+  <si>
+    <t>Ava</t>
   </si>
   <si>
     <t>Nutella</t>
   </si>
   <si>
     <t>Tasty</t>
-  </si>
-  <si>
-    <t>Farmer</t>
-  </si>
-  <si>
-    <t>Colgate</t>
-  </si>
-  <si>
-    <t>Kelloggs</t>
-  </si>
-  <si>
-    <t>Dixan</t>
-  </si>
-  <si>
-    <t>3 Άλφα</t>
-  </si>
-  <si>
-    <t>Παπαγάλος</t>
-  </si>
-  <si>
-    <t>Ava</t>
   </si>
   <si>
     <t>Royal Dutch</t>
@@ -775,7 +775,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4">
         <v>43998</v>
@@ -790,16 +790,16 @@
         <v>48</v>
       </c>
       <c r="G3" s="2">
-        <v>3.98</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="H3" s="2">
-        <v>0</v>
+        <v>5.59</v>
       </c>
       <c r="I3" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4">
         <v>43998</v>
@@ -895,16 +895,16 @@
         <v>51</v>
       </c>
       <c r="G6" s="2">
-        <v>1.55</v>
+        <v>3.98</v>
       </c>
       <c r="H6" s="2">
-        <v>1.15</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4">
         <v>43998</v>
@@ -930,22 +930,22 @@
         <v>52</v>
       </c>
       <c r="G7" s="2">
-        <v>8.949999999999999</v>
+        <v>3.98</v>
       </c>
       <c r="H7" s="2">
-        <v>5.59</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -965,22 +965,22 @@
         <v>53</v>
       </c>
       <c r="G8" s="2">
-        <v>3.78</v>
+        <v>5.95</v>
       </c>
       <c r="H8" s="2">
-        <v>2.95</v>
+        <v>5.59</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K8" s="1">
         <v>1</v>
       </c>
       <c r="L8" s="2">
-        <v>2.61</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1000,27 +1000,27 @@
         <v>54</v>
       </c>
       <c r="G9" s="2">
-        <v>1.7</v>
+        <v>5.95</v>
       </c>
       <c r="H9" s="2">
-        <v>1.3</v>
+        <v>5.59</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K9" s="1">
         <v>1</v>
       </c>
       <c r="L9" s="2">
-        <v>1.15</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="4">
         <v>43998</v>
@@ -1035,22 +1035,22 @@
         <v>55</v>
       </c>
       <c r="G10" s="2">
-        <v>5.95</v>
+        <v>3.98</v>
       </c>
       <c r="H10" s="2">
-        <v>5.59</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K10" s="1">
         <v>1</v>
       </c>
       <c r="L10" s="2">
-        <v>3.83</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1070,7 +1070,7 @@
         <v>56</v>
       </c>
       <c r="G11" s="2">
-        <v>5.95</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="H11" s="2">
         <v>5.59</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K11" s="1">
         <v>1</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4">
         <v>43998</v>
@@ -1105,22 +1105,22 @@
         <v>57</v>
       </c>
       <c r="G12" s="2">
-        <v>1.75</v>
+        <v>2.99</v>
       </c>
       <c r="H12" s="2">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K12" s="1">
         <v>1</v>
       </c>
       <c r="L12" s="2">
-        <v>0.88</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1140,22 +1140,22 @@
         <v>58</v>
       </c>
       <c r="G13" s="2">
-        <v>8.949999999999999</v>
+        <v>1.55</v>
       </c>
       <c r="H13" s="2">
-        <v>5.59</v>
+        <v>1.15</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K13" s="1">
         <v>1</v>
       </c>
       <c r="L13" s="2">
-        <v>4.51</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1175,27 +1175,27 @@
         <v>59</v>
       </c>
       <c r="G14" s="2">
-        <v>3.98</v>
+        <v>2.99</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="2">
-        <v>2.25</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" s="4">
         <v>43998</v>
@@ -1210,22 +1210,22 @@
         <v>60</v>
       </c>
       <c r="G15" s="2">
-        <v>2.99</v>
+        <v>1.75</v>
       </c>
       <c r="H15" s="2">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="I15" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="2">
-        <v>1.21</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1245,27 +1245,27 @@
         <v>61</v>
       </c>
       <c r="G16" s="2">
-        <v>3.98</v>
+        <v>4.3</v>
       </c>
       <c r="H16" s="2">
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="K16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="2">
-        <v>1.91</v>
+        <v>3.82</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4">
         <v>43998</v>
@@ -1280,22 +1280,22 @@
         <v>62</v>
       </c>
       <c r="G17" s="2">
-        <v>3.98</v>
+        <v>1.55</v>
       </c>
       <c r="H17" s="2">
-        <v>0</v>
+        <v>1.15</v>
       </c>
       <c r="I17" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K17" s="1">
         <v>2</v>
       </c>
       <c r="L17" s="2">
-        <v>4.5</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1315,22 +1315,22 @@
         <v>63</v>
       </c>
       <c r="G18" s="2">
-        <v>4.3</v>
+        <v>3.35</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
       </c>
       <c r="I18" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K18" s="1">
         <v>2</v>
       </c>
       <c r="L18" s="2">
-        <v>3.82</v>
+        <v>4.59</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1385,22 +1385,22 @@
         <v>65</v>
       </c>
       <c r="G20" s="2">
-        <v>2.99</v>
+        <v>3.98</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
       <c r="I20" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="K20" s="1">
         <v>2</v>
       </c>
       <c r="L20" s="2">
-        <v>2.42</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1420,7 +1420,7 @@
         <v>66</v>
       </c>
       <c r="G21" s="2">
-        <v>3.35</v>
+        <v>3.98</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -1429,18 +1429,18 @@
         <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K21" s="1">
         <v>2</v>
       </c>
       <c r="L21" s="2">
-        <v>3.78</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="4">
         <v>43998</v>
@@ -1455,27 +1455,27 @@
         <v>67</v>
       </c>
       <c r="G22" s="2">
-        <v>1.55</v>
+        <v>3.35</v>
       </c>
       <c r="H22" s="2">
-        <v>1.15</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>82</v>
       </c>
       <c r="K22" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L22" s="2">
-        <v>1.86</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" s="4">
         <v>43998</v>
@@ -1490,22 +1490,22 @@
         <v>68</v>
       </c>
       <c r="G23" s="2">
-        <v>3.35</v>
+        <v>3.45</v>
       </c>
       <c r="H23" s="2">
-        <v>0</v>
+        <v>1.69</v>
       </c>
       <c r="I23" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="K23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L23" s="2">
-        <v>4.59</v>
+        <v>4.49</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1525,7 +1525,7 @@
         <v>69</v>
       </c>
       <c r="G24" s="2">
-        <v>3.98</v>
+        <v>7.95</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
@@ -1534,13 +1534,13 @@
         <v>30</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="K24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L24" s="2">
-        <v>4.5</v>
+        <v>13.47</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1569,18 +1569,18 @@
         <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L25" s="2">
-        <v>8.98</v>
+        <v>13.47</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="4">
         <v>43998</v>
@@ -1595,27 +1595,27 @@
         <v>71</v>
       </c>
       <c r="G26" s="2">
-        <v>3.45</v>
+        <v>2.95</v>
       </c>
       <c r="H26" s="2">
-        <v>1.69</v>
+        <v>0</v>
       </c>
       <c r="I26" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="K26" s="1">
         <v>3</v>
       </c>
       <c r="L26" s="2">
-        <v>4.49</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" s="4">
         <v>43998</v>
@@ -1633,24 +1633,24 @@
         <v>2.95</v>
       </c>
       <c r="H27" s="2">
-        <v>0</v>
+        <v>2.29</v>
       </c>
       <c r="I27" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K27" s="1">
         <v>3</v>
       </c>
       <c r="L27" s="2">
-        <v>3.57</v>
+        <v>6.09</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="4">
         <v>43998</v>
@@ -1665,27 +1665,27 @@
         <v>73</v>
       </c>
       <c r="G28" s="2">
-        <v>7.95</v>
+        <v>1.55</v>
       </c>
       <c r="H28" s="2">
-        <v>0</v>
+        <v>1.15</v>
       </c>
       <c r="I28" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K28" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L28" s="2">
-        <v>13.47</v>
+        <v>3.72</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" s="4">
         <v>43998</v>
@@ -1700,22 +1700,22 @@
         <v>74</v>
       </c>
       <c r="G29" s="2">
-        <v>2.95</v>
+        <v>1.2</v>
       </c>
       <c r="H29" s="2">
-        <v>2.29</v>
+        <v>0</v>
       </c>
       <c r="I29" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K29" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L29" s="2">
-        <v>6.09</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1735,22 +1735,22 @@
         <v>75</v>
       </c>
       <c r="G30" s="2">
-        <v>1.55</v>
+        <v>3.78</v>
       </c>
       <c r="H30" s="2">
-        <v>1.15</v>
+        <v>2.95</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="K30" s="1">
         <v>4</v>
       </c>
       <c r="L30" s="2">
-        <v>3.72</v>
+        <v>10.44</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1779,18 +1779,18 @@
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K31" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L31" s="2">
-        <v>2.72</v>
+        <v>5.33</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C32" s="4">
         <v>43998</v>
@@ -1805,22 +1805,22 @@
         <v>77</v>
       </c>
       <c r="G32" s="2">
-        <v>1.2</v>
+        <v>1.7</v>
       </c>
       <c r="H32" s="2">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="I32" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K32" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L32" s="2">
-        <v>3.97</v>
+        <v>10.35</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1849,7 +1849,7 @@
         <v>50</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K33" s="1">
         <v>11</v>
@@ -1887,18 +1887,18 @@
         <v>93</v>
       </c>
       <c r="K34" s="1">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="L34" s="2">
-        <v>32.47</v>
+        <v>35.81</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="K35" s="5">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="L35" s="5">
-        <v>145.04</v>
+        <v>174.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>